<commit_message>
New post on xgb binning
</commit_message>
<xml_diff>
--- a/series_tracker.xlsx
+++ b/series_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D91726B-731B-4792-98E7-AC03A997B558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93CFC21-611E-4BD3-A3AC-DCEE81D3A612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23040" windowHeight="12204" xr2:uid="{667D72D7-C7EA-48E0-9147-BAF6BF452800}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{667D72D7-C7EA-48E0-9147-BAF6BF452800}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Blog Post</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Covid visualisation using leaflet</t>
+  </si>
+  <si>
+    <t>Monotonic binning using XGBOOST</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199B1233-9445-4211-9E56-71E3604D18DF}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,27 +475,35 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New post on PSO
</commit_message>
<xml_diff>
--- a/series_tracker.xlsx
+++ b/series_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE187ED-8E1F-47A5-9AD4-DEE0EB16E83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E9B90A-2FE5-4BF0-B091-E7AE54AAEB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{667D72D7-C7EA-48E0-9147-BAF6BF452800}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Blog Post</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Score reliability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSO optimisation </t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -430,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199B1233-9445-4211-9E56-71E3604D18DF}">
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,6 +529,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New post on MBO
</commit_message>
<xml_diff>
--- a/series_tracker.xlsx
+++ b/series_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E9B90A-2FE5-4BF0-B091-E7AE54AAEB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356AE7F1-9844-41EB-8380-6952E13157BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{667D72D7-C7EA-48E0-9147-BAF6BF452800}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Blog Post</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Bayesian Optimisation for XGBOOST</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199B1233-9445-4211-9E56-71E3604D18DF}">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,6 +543,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
post on correlated random variables
</commit_message>
<xml_diff>
--- a/series_tracker.xlsx
+++ b/series_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7693C893-BDD3-4F50-AA5E-EF136628BA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C756D2-FB75-4F8B-AA7B-5457C010BA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{667D72D7-C7EA-48E0-9147-BAF6BF452800}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Cutoff analysis</t>
   </si>
   <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
     <t>Covid visualisation using leaflet</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Reticulate</t>
+  </si>
+  <si>
+    <t>Loan portfolio optimisation</t>
   </si>
 </sst>
 </file>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{199B1233-9445-4211-9E56-71E3604D18DF}">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +470,7 @@
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -492,7 +492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -503,9 +503,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -514,9 +514,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -525,20 +525,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -547,54 +544,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>